<commit_message>
re-running university responses/police actions analyses
</commit_message>
<xml_diff>
--- a/docs/data-cleaning-requests/university_police_actions/university_police_actions_Canada.xlsx
+++ b/docs/data-cleaning-requests/university_police_actions/university_police_actions_Canada.xlsx
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B13">
-        <v>4942</v>
+        <v>4984</v>
       </c>
     </row>
     <row r="14">
@@ -560,7 +560,7 @@
         <v>22</v>
       </c>
       <c r="E2">
-        <v>0.004100652376514445</v>
+        <v>0.004068799704087294</v>
       </c>
     </row>
     <row r="3">
@@ -583,7 +583,7 @@
         <v>45</v>
       </c>
       <c r="E3">
-        <v>0.008387698042870456</v>
+        <v>0.008322544849269465</v>
       </c>
     </row>
     <row r="4">
@@ -606,7 +606,7 @@
         <v>17</v>
       </c>
       <c r="E4">
-        <v>0.003168685927306617</v>
+        <v>0.003144072498612909</v>
       </c>
     </row>
     <row r="5">
@@ -629,7 +629,7 @@
         <v>63</v>
       </c>
       <c r="E5">
-        <v>0.01174277726001864</v>
+        <v>0.01165156278897725</v>
       </c>
     </row>
     <row r="6">
@@ -652,7 +652,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="7">
@@ -675,7 +675,7 @@
         <v>18</v>
       </c>
       <c r="E7">
-        <v>0.003355079217148183</v>
+        <v>0.003329017939707786</v>
       </c>
     </row>
     <row r="8">
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="E8">
-        <v>0.0003727865796831314</v>
+        <v>0.000369890882189754</v>
       </c>
     </row>
     <row r="9">
@@ -721,7 +721,7 @@
         <v>24</v>
       </c>
       <c r="E9">
-        <v>0.004473438956197577</v>
+        <v>0.004438690586277048</v>
       </c>
     </row>
     <row r="10">
@@ -744,7 +744,7 @@
         <v>21</v>
       </c>
       <c r="E10">
-        <v>0.00391425908667288</v>
+        <v>0.003883854262992417</v>
       </c>
     </row>
     <row r="11">
@@ -767,7 +767,7 @@
         <v>32</v>
       </c>
       <c r="E11">
-        <v>0.005964585274930103</v>
+        <v>0.005918254115036064</v>
       </c>
     </row>
     <row r="12">
@@ -790,7 +790,7 @@
         <v>22</v>
       </c>
       <c r="E12">
-        <v>0.004100652376514445</v>
+        <v>0.004068799704087294</v>
       </c>
     </row>
     <row r="13">
@@ -813,7 +813,7 @@
         <v>30</v>
       </c>
       <c r="E13">
-        <v>0.005591798695246971</v>
+        <v>0.005548363232846311</v>
       </c>
     </row>
     <row r="14">
@@ -836,7 +836,7 @@
         <v>57</v>
       </c>
       <c r="E14">
-        <v>0.01062441752096925</v>
+        <v>0.01054189014240799</v>
       </c>
     </row>
     <row r="15">
@@ -859,7 +859,7 @@
         <v>89</v>
       </c>
       <c r="E15">
-        <v>0.01658900279589935</v>
+        <v>0.01646014425744406</v>
       </c>
     </row>
     <row r="16">
@@ -882,7 +882,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="17">
@@ -905,7 +905,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="18">
@@ -928,7 +928,7 @@
         <v>13</v>
       </c>
       <c r="E18">
-        <v>0.002423112767940354</v>
+        <v>0.002404290734233401</v>
       </c>
     </row>
     <row r="19">
@@ -951,7 +951,7 @@
         <v>15</v>
       </c>
       <c r="E19">
-        <v>0.002795899347623486</v>
+        <v>0.002774181616423155</v>
       </c>
     </row>
     <row r="20">
@@ -974,7 +974,7 @@
         <v>14</v>
       </c>
       <c r="E20">
-        <v>0.00260950605778192</v>
+        <v>0.002589236175328278</v>
       </c>
     </row>
     <row r="21">
@@ -997,7 +997,7 @@
         <v>17</v>
       </c>
       <c r="E21">
-        <v>0.003168685927306617</v>
+        <v>0.003144072498612909</v>
       </c>
     </row>
     <row r="22">
@@ -1020,7 +1020,7 @@
         <v>125</v>
       </c>
       <c r="E22">
-        <v>0.02329916123019571</v>
+        <v>0.02311818013685963</v>
       </c>
     </row>
     <row r="23">
@@ -1043,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="E23">
-        <v>0.004100652376514445</v>
+        <v>0.004068799704087294</v>
       </c>
     </row>
     <row r="24">
@@ -1066,7 +1066,7 @@
         <v>27</v>
       </c>
       <c r="E24">
-        <v>0.005032618825722274</v>
+        <v>0.004993526909561679</v>
       </c>
     </row>
     <row r="25">
@@ -1089,7 +1089,7 @@
         <v>52</v>
       </c>
       <c r="E25">
-        <v>0.009692451071761416</v>
+        <v>0.009617162936933604</v>
       </c>
     </row>
     <row r="26">
@@ -1112,7 +1112,7 @@
         <v>102</v>
       </c>
       <c r="E26">
-        <v>0.0190121155638397</v>
+        <v>0.01886443499167745</v>
       </c>
     </row>
     <row r="27">
@@ -1135,7 +1135,7 @@
         <v>59</v>
       </c>
       <c r="E27">
-        <v>0.01099720410065238</v>
+        <v>0.01091178102459774</v>
       </c>
     </row>
     <row r="28">
@@ -1158,7 +1158,7 @@
         <v>11</v>
       </c>
       <c r="E28">
-        <v>0.002050326188257223</v>
+        <v>0.002034399852043647</v>
       </c>
     </row>
     <row r="29">
@@ -1181,7 +1181,7 @@
         <v>70</v>
       </c>
       <c r="E29">
-        <v>0.0130475302889096</v>
+        <v>0.01294618087664139</v>
       </c>
     </row>
     <row r="30">
@@ -1204,7 +1204,7 @@
         <v>22</v>
       </c>
       <c r="E30">
-        <v>0.004100652376514445</v>
+        <v>0.004068799704087294</v>
       </c>
     </row>
     <row r="31">
@@ -1227,7 +1227,7 @@
         <v>59</v>
       </c>
       <c r="E31">
-        <v>0.01099720410065238</v>
+        <v>0.01091178102459774</v>
       </c>
     </row>
     <row r="32">
@@ -1250,7 +1250,7 @@
         <v>2</v>
       </c>
       <c r="E32">
-        <v>0.0003727865796831314</v>
+        <v>0.000369890882189754</v>
       </c>
     </row>
     <row r="33">
@@ -1273,7 +1273,7 @@
         <v>8</v>
       </c>
       <c r="E33">
-        <v>0.001491146318732526</v>
+        <v>0.001479563528759016</v>
       </c>
     </row>
     <row r="34">
@@ -1296,7 +1296,7 @@
         <v>7</v>
       </c>
       <c r="E34">
-        <v>0.00130475302889096</v>
+        <v>0.001294618087664139</v>
       </c>
     </row>
     <row r="35">
@@ -1319,7 +1319,7 @@
         <v>10</v>
       </c>
       <c r="E35">
-        <v>0.001863932898415657</v>
+        <v>0.00184945441094877</v>
       </c>
     </row>
     <row r="36">
@@ -1342,7 +1342,7 @@
         <v>4</v>
       </c>
       <c r="E36">
-        <v>0.0007455731593662628</v>
+        <v>0.0007397817643795081</v>
       </c>
     </row>
     <row r="37">
@@ -1365,7 +1365,7 @@
         <v>5</v>
       </c>
       <c r="E37">
-        <v>0.0009319664492078285</v>
+        <v>0.0009247272054743851</v>
       </c>
     </row>
     <row r="38">
@@ -1388,7 +1388,7 @@
         <v>29</v>
       </c>
       <c r="E38">
-        <v>0.005405405405405406</v>
+        <v>0.005363417791751433</v>
       </c>
     </row>
     <row r="39">
@@ -1411,7 +1411,7 @@
         <v>1</v>
       </c>
       <c r="E39">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="40">
@@ -1434,7 +1434,7 @@
         <v>4</v>
       </c>
       <c r="E40">
-        <v>0.0007455731593662628</v>
+        <v>0.0007397817643795081</v>
       </c>
     </row>
     <row r="41">
@@ -1457,7 +1457,7 @@
         <v>3</v>
       </c>
       <c r="E41">
-        <v>0.0005591798695246971</v>
+        <v>0.000554836323284631</v>
       </c>
     </row>
     <row r="42">
@@ -1480,7 +1480,7 @@
         <v>9</v>
       </c>
       <c r="E42">
-        <v>0.001677539608574091</v>
+        <v>0.001664508969853893</v>
       </c>
     </row>
     <row r="43">
@@ -1503,7 +1503,7 @@
         <v>5</v>
       </c>
       <c r="E43">
-        <v>0.0009319664492078285</v>
+        <v>0.0009247272054743851</v>
       </c>
     </row>
     <row r="44">
@@ -1526,7 +1526,7 @@
         <v>5</v>
       </c>
       <c r="E44">
-        <v>0.0009319664492078285</v>
+        <v>0.0009247272054743851</v>
       </c>
     </row>
     <row r="45">
@@ -1549,7 +1549,7 @@
         <v>3</v>
       </c>
       <c r="E45">
-        <v>0.0005591798695246971</v>
+        <v>0.000554836323284631</v>
       </c>
     </row>
     <row r="46">
@@ -1572,7 +1572,7 @@
         <v>3</v>
       </c>
       <c r="E46">
-        <v>0.0005591798695246971</v>
+        <v>0.000554836323284631</v>
       </c>
     </row>
     <row r="47">
@@ -1595,7 +1595,7 @@
         <v>106</v>
       </c>
       <c r="E47">
-        <v>0.01975768872320597</v>
+        <v>0.01960421675605696</v>
       </c>
     </row>
     <row r="48">
@@ -1618,7 +1618,7 @@
         <v>25</v>
       </c>
       <c r="E48">
-        <v>0.004659832246039142</v>
+        <v>0.004623636027371925</v>
       </c>
     </row>
     <row r="49">
@@ -1641,7 +1641,7 @@
         <v>54</v>
       </c>
       <c r="E49">
-        <v>0.01006523765144455</v>
+        <v>0.009987053819123359</v>
       </c>
     </row>
     <row r="50">
@@ -1664,7 +1664,7 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="51">
@@ -1687,7 +1687,7 @@
         <v>1</v>
       </c>
       <c r="E51">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="52">
@@ -1710,7 +1710,7 @@
         <v>25</v>
       </c>
       <c r="E52">
-        <v>0.004659832246039142</v>
+        <v>0.004623636027371925</v>
       </c>
     </row>
     <row r="53">
@@ -1733,7 +1733,7 @@
         <v>29</v>
       </c>
       <c r="E53">
-        <v>0.005405405405405406</v>
+        <v>0.005363417791751433</v>
       </c>
     </row>
     <row r="54">
@@ -1756,7 +1756,7 @@
         <v>8</v>
       </c>
       <c r="E54">
-        <v>0.001491146318732526</v>
+        <v>0.001479563528759016</v>
       </c>
     </row>
     <row r="55">
@@ -1779,7 +1779,7 @@
         <v>31</v>
       </c>
       <c r="E55">
-        <v>0.005778191985088537</v>
+        <v>0.005733308673941187</v>
       </c>
     </row>
     <row r="56">
@@ -1802,7 +1802,7 @@
         <v>37</v>
       </c>
       <c r="E56">
-        <v>0.006896551724137931</v>
+        <v>0.006842981320510449</v>
       </c>
     </row>
     <row r="57">
@@ -1825,7 +1825,7 @@
         <v>23</v>
       </c>
       <c r="E57">
-        <v>0.004287045666356011</v>
+        <v>0.004253745145182172</v>
       </c>
     </row>
     <row r="58">
@@ -1848,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>0.0001863932898415657</v>
+        <v>0.000184945441094877</v>
       </c>
     </row>
     <row r="59">
@@ -1871,7 +1871,7 @@
         <v>20</v>
       </c>
       <c r="E59">
-        <v>0.003727865796831314</v>
+        <v>0.00369890882189754</v>
       </c>
     </row>
     <row r="60">
@@ -1894,7 +1894,7 @@
         <v>20</v>
       </c>
       <c r="E60">
-        <v>0.003727865796831314</v>
+        <v>0.00369890882189754</v>
       </c>
     </row>
     <row r="61">
@@ -1917,7 +1917,7 @@
         <v>19</v>
       </c>
       <c r="E61">
-        <v>0.003541472506989748</v>
+        <v>0.003513963380802663</v>
       </c>
     </row>
     <row r="62">
@@ -1940,7 +1940,7 @@
         <v>4</v>
       </c>
       <c r="E62">
-        <v>0.0007455731593662628</v>
+        <v>0.0007397817643795081</v>
       </c>
     </row>
     <row r="63">
@@ -1963,7 +1963,7 @@
         <v>31</v>
       </c>
       <c r="E63">
-        <v>0.005778191985088537</v>
+        <v>0.005733308673941187</v>
       </c>
     </row>
     <row r="64">
@@ -1986,7 +1986,7 @@
         <v>4</v>
       </c>
       <c r="E64">
-        <v>0.0007455731593662628</v>
+        <v>0.0007397817643795081</v>
       </c>
     </row>
     <row r="65">
@@ -2009,7 +2009,7 @@
         <v>27</v>
       </c>
       <c r="E65">
-        <v>0.005032618825722274</v>
+        <v>0.004993526909561679</v>
       </c>
     </row>
     <row r="66">
@@ -2032,7 +2032,7 @@
         <v>26</v>
       </c>
       <c r="E66">
-        <v>0.004846225535880708</v>
+        <v>0.004808581468466802</v>
       </c>
     </row>
     <row r="67">
@@ -2055,7 +2055,7 @@
         <v>27</v>
       </c>
       <c r="E67">
-        <v>0.005032618825722274</v>
+        <v>0.004993526909561679</v>
       </c>
     </row>
     <row r="68">
@@ -2078,7 +2078,7 @@
         <v>31</v>
       </c>
       <c r="E68">
-        <v>0.005778191985088537</v>
+        <v>0.005733308673941187</v>
       </c>
     </row>
     <row r="69">
@@ -2101,7 +2101,7 @@
         <v>24</v>
       </c>
       <c r="E69">
-        <v>0.004473438956197577</v>
+        <v>0.004438690586277048</v>
       </c>
     </row>
     <row r="70">
@@ -2124,7 +2124,7 @@
         <v>10</v>
       </c>
       <c r="E70">
-        <v>0.001863932898415657</v>
+        <v>0.00184945441094877</v>
       </c>
     </row>
     <row r="71">
@@ -2147,7 +2147,7 @@
         <v>16</v>
       </c>
       <c r="E71">
-        <v>0.002982292637465051</v>
+        <v>0.002959127057518032</v>
       </c>
     </row>
     <row r="72">
@@ -2170,7 +2170,7 @@
         <v>2</v>
       </c>
       <c r="E72">
-        <v>0.0003727865796831314</v>
+        <v>0.000369890882189754</v>
       </c>
     </row>
     <row r="73">
@@ -2193,7 +2193,7 @@
         <v>9</v>
       </c>
       <c r="E73">
-        <v>0.001677539608574091</v>
+        <v>0.001664508969853893</v>
       </c>
     </row>
     <row r="74">

</xml_diff>